<commit_message>
[IMP] z0bug_odoo: new test data
</commit_message>
<xml_diff>
--- a/z0bug_odoo/build/lib.linux-x86_64-2.7/z0bug_odoo/data/account_tax.xlsx
+++ b/z0bug_odoo/build/lib.linux-x86_64-2.7/z0bug_odoo/data/account_tax.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="310">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -938,6 +938,9 @@
   </si>
   <si>
     <t xml:space="preserve">Art. 17ter - split-payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.coa_260060</t>
   </si>
   <si>
     <t xml:space="preserve">S</t>
@@ -1060,12 +1063,12 @@
   <dimension ref="A1:N89"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A89" activeCellId="0" sqref="A89"/>
+      <selection pane="bottomLeft" activeCell="M84" activeCellId="0" sqref="M84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
@@ -3623,21 +3626,21 @@
         <v>19</v>
       </c>
       <c r="I88" s="0" t="s">
-        <v>164</v>
+        <v>306</v>
       </c>
       <c r="J88" s="0" t="s">
-        <v>164</v>
+        <v>306</v>
       </c>
       <c r="N88" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>305</v>
@@ -3658,13 +3661,13 @@
         <v>19</v>
       </c>
       <c r="I89" s="0" t="s">
-        <v>164</v>
+        <v>306</v>
       </c>
       <c r="J89" s="0" t="s">
-        <v>164</v>
+        <v>306</v>
       </c>
       <c r="N89" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>